<commit_message>
fixed why 2023 acid digestions weren't merging properly
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2023_AcidDigestion_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2023_AcidDigestion_EDI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Documents/R/GitHub/Metals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{75890CF4-1953-FC4C-AA91-48567BF55C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD035BB5-47DF-034F-BEE3-441A3F430E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{09F8E85E-FD52-2D49-8A5D-8718B1783EFE}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15500" xr2:uid="{09F8E85E-FD52-2D49-8A5D-8718B1783EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="2023_AcidDigestion_EDI" sheetId="1" r:id="rId1"/>
@@ -53,1191 +53,783 @@
     <t>Filter2Mass_g</t>
   </si>
   <si>
-    <t>5_2023-04-24</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_24Apr23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_24Apr23</t>
   </si>
   <si>
-    <t>6_2023-04-24</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_24Apr23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_24Apr23</t>
   </si>
   <si>
-    <t>7_2023-04-24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_24Apr23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_24Apr23</t>
   </si>
   <si>
-    <t>8_2023-04-24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_24Apr23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_24Apr23</t>
   </si>
   <si>
-    <t>1_2023-05-01</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_01May23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_01May23</t>
   </si>
   <si>
-    <t>2_2023-05-01</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_01May23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_01May23</t>
   </si>
   <si>
-    <t>3_2023-05-01</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_01May23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_01May23</t>
   </si>
   <si>
-    <t>4_2023-05-01</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_01May23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_01May23</t>
   </si>
   <si>
-    <t>1_2023-05-08</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_08May23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_08May23</t>
   </si>
   <si>
-    <t>2_2023-05-08</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_08May23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_08May23</t>
   </si>
   <si>
-    <t>3_2023-05-08</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_08May23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_08May23</t>
   </si>
   <si>
-    <t>4_2023-05-08</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_08May23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_08May23</t>
   </si>
   <si>
-    <t>5_2022-05-08</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_08May22</t>
   </si>
   <si>
-    <t>6_2023-05-08</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_08May23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_08May23</t>
   </si>
   <si>
-    <t>7_2023-05-08</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_08May23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_08May23</t>
   </si>
   <si>
-    <t>8_2023-05-08</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_08May23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_08May23</t>
   </si>
   <si>
-    <t>1_2023-05-22</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_22May23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_22May23</t>
   </si>
   <si>
-    <t>2_2023-05-22</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_22May23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_22May23</t>
   </si>
   <si>
-    <t>3_2023-05-22</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_22May23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_22May23</t>
   </si>
   <si>
-    <t>4_2023-05-22</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_22May23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_22May23</t>
   </si>
   <si>
-    <t>5_2023-05-22</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_22May23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_22May23</t>
   </si>
   <si>
-    <t>6_2023-05-22</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_22May23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_22May23</t>
   </si>
   <si>
-    <t>7_2023-05-22</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_22May23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_22May23</t>
   </si>
   <si>
-    <t>8_2023-05-22</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_22May23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_22May23</t>
   </si>
   <si>
-    <t>1_2023-06-05</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_05Jun23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_05Jun23</t>
   </si>
   <si>
-    <t>2_2023-06-05</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_05Jun23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_05Jun23</t>
   </si>
   <si>
-    <t>3_2023-06-05</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_05Jun23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_05Jun23</t>
   </si>
   <si>
-    <t>4_2023-06-05</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_05Jun23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_05Jun23</t>
   </si>
   <si>
-    <t>5_2023-06-05</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_05Jun23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_05Jun23</t>
   </si>
   <si>
-    <t>6_2023-06-05</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_05Jun23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_05Jun23</t>
   </si>
   <si>
-    <t>7_2023-06-05</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_05Jun23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_05Jun23</t>
   </si>
   <si>
-    <t>8_2023-06-05</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_05Jun23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_05Jun23</t>
   </si>
   <si>
-    <t>1_2023-06-19</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_19Jun23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_19Jun23</t>
   </si>
   <si>
-    <t>2_2023-06-19</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_19Jun23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_19Jun23</t>
   </si>
   <si>
-    <t>3_2023-06-19</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_19Jun23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_19Jun23</t>
   </si>
   <si>
-    <t>4_2023-06-19</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_19Jun23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_19Jun23</t>
   </si>
   <si>
-    <t>5_2023-06-19</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_19Jun23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_19Jun23</t>
   </si>
   <si>
-    <t>6_2023-06-19</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_19Jun23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_19Jun23</t>
   </si>
   <si>
-    <t>7_2023-06-19</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_19Jun23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_19Jun23</t>
   </si>
   <si>
-    <t>8_2023-06-19</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_19Jun23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_19Jun23</t>
   </si>
   <si>
-    <t>1_2023-07-03</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_03Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_03Jul23</t>
   </si>
   <si>
-    <t>2_2023-07-03</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_03Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_03Jul23</t>
   </si>
   <si>
-    <t>3_2023-07-03</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_03Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_03Jul23</t>
   </si>
   <si>
-    <t>4_2023-07-03</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_03Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_03Jul23</t>
   </si>
   <si>
-    <t>5_2023-07-03</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_03Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_03Jul23</t>
   </si>
   <si>
-    <t>6_2023-07-03</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_03Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_03Jul23</t>
   </si>
   <si>
-    <t>7_2023-07-03</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_03Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_03Jul23</t>
   </si>
   <si>
-    <t>8_2023-07-03</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_03Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_03Jul23</t>
   </si>
   <si>
-    <t>1_2023-07-17</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_17Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_17Jul23</t>
   </si>
   <si>
-    <t>2_2023-07-17</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_17Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_17Jul23</t>
   </si>
   <si>
-    <t>3_2023-07-17</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_17Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_17Jul23</t>
   </si>
   <si>
-    <t>4_2023-07-17</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_17Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_17Jul23</t>
   </si>
   <si>
-    <t>5_2023-07-17</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_17Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_17Jul23</t>
   </si>
   <si>
-    <t>6_2023-07-17</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_17Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_17Jul23</t>
   </si>
   <si>
-    <t>7_2023-07-17</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_17Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_17Jul23</t>
   </si>
   <si>
-    <t>8_2023-07-17</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_17Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_17Jul23</t>
   </si>
   <si>
-    <t>1_2023-07-31</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_31Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_31Jul23</t>
   </si>
   <si>
-    <t>2_2023-07-31</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_31Jul23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_31Jul23</t>
   </si>
   <si>
-    <t>3_2023-07-31</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_31Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_31Jul23</t>
   </si>
   <si>
-    <t>4_2023-07-31</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_31Jul23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_31Jul23</t>
   </si>
   <si>
-    <t>5_2023-07-31</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_31Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_31Jul23</t>
   </si>
   <si>
-    <t>6_2023-07-31</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_31Jul23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_31Jul23</t>
   </si>
   <si>
-    <t>7_2023-07-31</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_31Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_31Jul23</t>
   </si>
   <si>
-    <t>8_2023-07-31</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_31Jul23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_31Jul23</t>
   </si>
   <si>
-    <t>1_2023-08-14</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_14Aug23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_14Aug23</t>
   </si>
   <si>
-    <t>2_2023-08-14</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_14Aug23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_14Aug23</t>
   </si>
   <si>
-    <t>3_2023-08-14</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_14Aug23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_14Aug23</t>
   </si>
   <si>
-    <t>4_2023-08-14</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_14Aug23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_14Aug23</t>
   </si>
   <si>
-    <t>5_2023-08-14</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_14Aug23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_14Aug23</t>
   </si>
   <si>
-    <t>6_2023-08-14</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_14Aug23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_14Aug23</t>
   </si>
   <si>
-    <t>7_2023-08-14</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_14Aug23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_14Aug23</t>
   </si>
   <si>
-    <t>8_2023-08-14</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_14Aug23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_14Aug23</t>
   </si>
   <si>
-    <t>1_2023-08-29</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_29Aug23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_29Aug23</t>
   </si>
   <si>
-    <t>2_2023-08-29</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_29Aug23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_29Aug23</t>
   </si>
   <si>
-    <t>3_2023-08-29</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_29Aug23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_29Aug23</t>
   </si>
   <si>
-    <t>4_2023-08-29</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_29Aug23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_29Aug23</t>
   </si>
   <si>
-    <t>5_2023-08-29</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_29Aug23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_29Aug23</t>
   </si>
   <si>
-    <t>6_2023-08-29</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_29Aug23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_29Aug23</t>
   </si>
   <si>
-    <t>7_2023-08-29</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_29Aug23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_29Aug23</t>
   </si>
   <si>
-    <t>8_2023-08-29</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_29Aug23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_29Aug23</t>
   </si>
   <si>
-    <t>1_2023-09-12</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_12Sep23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_12Sep23</t>
   </si>
   <si>
-    <t>2_2023-09-12</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_12Sep23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_12Sep23</t>
   </si>
   <si>
-    <t>3_2023-09-12</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_12Sep23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_12Sep23</t>
   </si>
   <si>
-    <t>4_2023-09-12</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_12Sep23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_12Sep23</t>
   </si>
   <si>
-    <t>5_2023-09-12</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_12Sep23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_12Sep23</t>
   </si>
   <si>
-    <t>6_2023-09-12</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_12Sep23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_12Sep23</t>
   </si>
   <si>
-    <t>7_2023-09-12</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_12Sep23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_12Sep23</t>
   </si>
   <si>
-    <t>8_2023-09-12</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_12Sep23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_12Sep23</t>
   </si>
   <si>
-    <t>1_2023-09-25</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_25Sep23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_25Sep23</t>
   </si>
   <si>
-    <t>2_2023-09-25</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_25Sep23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_25Sep23</t>
   </si>
   <si>
-    <t>3_2023-09-25</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_25Sep23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_25Sep23</t>
   </si>
   <si>
-    <t>4_2023-09-25</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_25Sep23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_25Sep23</t>
   </si>
   <si>
-    <t>5_2023-09-26</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_26Sep23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_26Sep23</t>
   </si>
   <si>
-    <t>6_2023-09-26</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_26Sep23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_26Sep23</t>
   </si>
   <si>
-    <t>7_2023-09-26</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_26Sep23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_26Sep23</t>
   </si>
   <si>
-    <t>8_2023-09-26</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_26Sep23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_26Sep23</t>
   </si>
   <si>
-    <t>1_2023-10-09</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_09Oct23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_09Oct23</t>
   </si>
   <si>
-    <t>2_2023-10-09</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_09Oct23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_09Oct23</t>
   </si>
   <si>
-    <t>3_2023-10-09</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_09Oct23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_09Oct23</t>
   </si>
   <si>
-    <t>4_2023-10-09</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_09Oct23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_09Oct23</t>
   </si>
   <si>
-    <t>5_2023-10-09</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_09Oct23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_09Oct23</t>
   </si>
   <si>
-    <t>6_2023-10-09</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_09Oct23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_09Oct23</t>
   </si>
   <si>
-    <t>7_2023-10-09</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_09Oct23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_09Oct23</t>
   </si>
   <si>
-    <t>8_2023-10-09</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_09Oct23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_09Oct23</t>
   </si>
   <si>
-    <t>1_2023-10-24</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_24Oct23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_24Oct23</t>
   </si>
   <si>
-    <t>2_2023-10-24</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_24Oct23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_24Oct23</t>
   </si>
   <si>
-    <t>3_2023-10-24</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_24Oct23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_24Oct23</t>
   </si>
   <si>
-    <t>4_2023-10-24</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_24Oct23</t>
   </si>
   <si>
     <t>F_sed_8m_R2_F2_24Oct23</t>
   </si>
   <si>
-    <t>5_2023-10-24</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_24Oct23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_24Oct23</t>
   </si>
   <si>
-    <t>6_2023-10-24</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_24Oct23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_24Oct23</t>
   </si>
   <si>
-    <t>7_2023-10-24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_24Oct23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_24Oct23</t>
   </si>
   <si>
-    <t>8_2023-10-24</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_24Oct23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_24Oct23</t>
   </si>
   <si>
-    <t>1_2023-11-06</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_06Nov23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_06Nov23</t>
   </si>
   <si>
-    <t>2_2023-11-06</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_06Nov23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_06Nov23</t>
   </si>
   <si>
-    <t>3_2023-11-06</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_06Nov23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_06Nov23</t>
   </si>
   <si>
-    <t>4_2023-11-06</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_06Nov23</t>
   </si>
   <si>
-    <t>5_2023-11-06</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_06Nov23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_06Nov23</t>
   </si>
   <si>
-    <t>6_2023-11-06</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_06Nov23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_06Nov23</t>
   </si>
   <si>
-    <t>7_2023-11-06</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_06Nov23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_06Nov23</t>
   </si>
   <si>
-    <t>8_2023-11-06</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_06Nov23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_06Nov23</t>
   </si>
   <si>
-    <t>1_2023-11-17</t>
-  </si>
-  <si>
     <t>F_sed_4m_R1_F1_17Nov23</t>
   </si>
   <si>
     <t>F_sed_4m_R1_F2_17Nov23</t>
   </si>
   <si>
-    <t>2_2023-11-17</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_17Nov23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_17Nov23</t>
   </si>
   <si>
-    <t>3_2023-11-17</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_17Nov23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_17Nov23</t>
   </si>
   <si>
-    <t>4_2023-11-17</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_17Nov23</t>
   </si>
   <si>
-    <t>5_2023-11-17</t>
-  </si>
-  <si>
     <t>B_sed_4m_R1_F1_17Nov23</t>
   </si>
   <si>
     <t>B_sed_4m_R1_F2_17Nov23</t>
   </si>
   <si>
-    <t>6_2023-11-17</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_17Nov23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_17Nov23</t>
   </si>
   <si>
-    <t>7_2023-11-17</t>
-  </si>
-  <si>
-    <t>8_2023-11-17</t>
-  </si>
-  <si>
-    <t>5_2023-12-04</t>
-  </si>
-  <si>
-    <t>6_2023-12-04</t>
-  </si>
-  <si>
     <t>B_sed_4m_R2_F1_04Dec23</t>
   </si>
   <si>
     <t>B_sed_4m_R2_F2_04Dec23</t>
   </si>
   <si>
-    <t>7_2023-12-04</t>
-  </si>
-  <si>
     <t>B_sed_8m_R1_F1_04Dec23</t>
   </si>
   <si>
     <t>B_sed_8m_R1_F2_04Dec23</t>
   </si>
   <si>
-    <t>8_2023-12-04</t>
-  </si>
-  <si>
     <t>B_sed_8m_R2_F1_04Dec23</t>
   </si>
   <si>
     <t>B_sed_8m_R2_F2_04Dec23</t>
   </si>
   <si>
-    <t>1_2023-12-04</t>
-  </si>
-  <si>
-    <t>2_2023-12-04</t>
-  </si>
-  <si>
     <t>F_sed_4m_R2_F1_04Dec23</t>
   </si>
   <si>
     <t>F_sed_4m_R2_F2_04Dec23</t>
   </si>
   <si>
-    <t>3_2023-12-04</t>
-  </si>
-  <si>
     <t>F_sed_8m_R1_F1_04Dec23</t>
   </si>
   <si>
     <t>F_sed_8m_R1_F2_04Dec23</t>
   </si>
   <si>
-    <t>4_2023-12-04</t>
-  </si>
-  <si>
     <t>F_sed_8m_R2_F1_04Dec23</t>
   </si>
   <si>
@@ -1296,6 +888,414 @@
   </si>
   <si>
     <t>F_sed_4m_R1_F3_04Dec23</t>
+  </si>
+  <si>
+    <t>5_24Apr23</t>
+  </si>
+  <si>
+    <t>6_24Apr23</t>
+  </si>
+  <si>
+    <t>7_24Apr23</t>
+  </si>
+  <si>
+    <t>8_24Apr23</t>
+  </si>
+  <si>
+    <t>1_01May23</t>
+  </si>
+  <si>
+    <t>2_01May23</t>
+  </si>
+  <si>
+    <t>3_01May23</t>
+  </si>
+  <si>
+    <t>4_01May23</t>
+  </si>
+  <si>
+    <t>1_08May23</t>
+  </si>
+  <si>
+    <t>2_08May23</t>
+  </si>
+  <si>
+    <t>3_08May23</t>
+  </si>
+  <si>
+    <t>4_08May23</t>
+  </si>
+  <si>
+    <t>5_08May23</t>
+  </si>
+  <si>
+    <t>6_08May23</t>
+  </si>
+  <si>
+    <t>7_08May23</t>
+  </si>
+  <si>
+    <t>8_08May23</t>
+  </si>
+  <si>
+    <t>1_22May23</t>
+  </si>
+  <si>
+    <t>2_22May23</t>
+  </si>
+  <si>
+    <t>3_22May23</t>
+  </si>
+  <si>
+    <t>4_22May23</t>
+  </si>
+  <si>
+    <t>5_22May23</t>
+  </si>
+  <si>
+    <t>6_22May23</t>
+  </si>
+  <si>
+    <t>7_22May23</t>
+  </si>
+  <si>
+    <t>8_22May23</t>
+  </si>
+  <si>
+    <t>1_05Jun23</t>
+  </si>
+  <si>
+    <t>2_05Jun23</t>
+  </si>
+  <si>
+    <t>3_05Jun23</t>
+  </si>
+  <si>
+    <t>4_05Jun23</t>
+  </si>
+  <si>
+    <t>5_05Jun23</t>
+  </si>
+  <si>
+    <t>6_05Jun23</t>
+  </si>
+  <si>
+    <t>7_05Jun23</t>
+  </si>
+  <si>
+    <t>8_05Jun23</t>
+  </si>
+  <si>
+    <t>1_19Jun23</t>
+  </si>
+  <si>
+    <t>2_19Jun23</t>
+  </si>
+  <si>
+    <t>3_19Jun23</t>
+  </si>
+  <si>
+    <t>4_19Jun23</t>
+  </si>
+  <si>
+    <t>5_19Jun23</t>
+  </si>
+  <si>
+    <t>6_19Jun23</t>
+  </si>
+  <si>
+    <t>7_19Jun23</t>
+  </si>
+  <si>
+    <t>8_19Jun23</t>
+  </si>
+  <si>
+    <t>1_03Jul23</t>
+  </si>
+  <si>
+    <t>2_03Jul23</t>
+  </si>
+  <si>
+    <t>3_03Jul23</t>
+  </si>
+  <si>
+    <t>4_03Jul23</t>
+  </si>
+  <si>
+    <t>5_03Jul23</t>
+  </si>
+  <si>
+    <t>6_03Jul23</t>
+  </si>
+  <si>
+    <t>7_03Jul23</t>
+  </si>
+  <si>
+    <t>8_03Jul23</t>
+  </si>
+  <si>
+    <t>1_17Jul23</t>
+  </si>
+  <si>
+    <t>2_17Jul23</t>
+  </si>
+  <si>
+    <t>3_17Jul23</t>
+  </si>
+  <si>
+    <t>4_17Jul23</t>
+  </si>
+  <si>
+    <t>5_17Jul23</t>
+  </si>
+  <si>
+    <t>6_17Jul23</t>
+  </si>
+  <si>
+    <t>7_17Jul23</t>
+  </si>
+  <si>
+    <t>8_17Jul23</t>
+  </si>
+  <si>
+    <t>1_31Jul23</t>
+  </si>
+  <si>
+    <t>2_31Jul23</t>
+  </si>
+  <si>
+    <t>3_31Jul23</t>
+  </si>
+  <si>
+    <t>4_31Jul23</t>
+  </si>
+  <si>
+    <t>5_31Jul23</t>
+  </si>
+  <si>
+    <t>6_31Jul23</t>
+  </si>
+  <si>
+    <t>7_31Jul23</t>
+  </si>
+  <si>
+    <t>8_31Jul23</t>
+  </si>
+  <si>
+    <t>1_14Aug23</t>
+  </si>
+  <si>
+    <t>2_14Aug23</t>
+  </si>
+  <si>
+    <t>3_14Aug23</t>
+  </si>
+  <si>
+    <t>4_14Aug23</t>
+  </si>
+  <si>
+    <t>5_14Aug23</t>
+  </si>
+  <si>
+    <t>6_14Aug23</t>
+  </si>
+  <si>
+    <t>7_14Aug23</t>
+  </si>
+  <si>
+    <t>8_14Aug23</t>
+  </si>
+  <si>
+    <t>1_29Aug23</t>
+  </si>
+  <si>
+    <t>2_29Aug23</t>
+  </si>
+  <si>
+    <t>3_29Aug23</t>
+  </si>
+  <si>
+    <t>4_29Aug23</t>
+  </si>
+  <si>
+    <t>5_29Aug23</t>
+  </si>
+  <si>
+    <t>6_29Aug23</t>
+  </si>
+  <si>
+    <t>7_29Aug23</t>
+  </si>
+  <si>
+    <t>8_29Aug23</t>
+  </si>
+  <si>
+    <t>1_12Sep23</t>
+  </si>
+  <si>
+    <t>2_12Sep23</t>
+  </si>
+  <si>
+    <t>3_12Sep23</t>
+  </si>
+  <si>
+    <t>4_12Sep23</t>
+  </si>
+  <si>
+    <t>5_12Sep23</t>
+  </si>
+  <si>
+    <t>6_12Sep23</t>
+  </si>
+  <si>
+    <t>7_12Sep23</t>
+  </si>
+  <si>
+    <t>8_12Sep23</t>
+  </si>
+  <si>
+    <t>1_25Sep23</t>
+  </si>
+  <si>
+    <t>2_25Sep23</t>
+  </si>
+  <si>
+    <t>3_25Sep23</t>
+  </si>
+  <si>
+    <t>4_25Sep23</t>
+  </si>
+  <si>
+    <t>6_26Sep23</t>
+  </si>
+  <si>
+    <t>5_26Sep23</t>
+  </si>
+  <si>
+    <t>7_26Sep23</t>
+  </si>
+  <si>
+    <t>8_26Sep23</t>
+  </si>
+  <si>
+    <t>1_09Oct23</t>
+  </si>
+  <si>
+    <t>2_09Oct23</t>
+  </si>
+  <si>
+    <t>3_09Oct23</t>
+  </si>
+  <si>
+    <t>4_09Oct23</t>
+  </si>
+  <si>
+    <t>5_09Oct23</t>
+  </si>
+  <si>
+    <t>6_09Oct23</t>
+  </si>
+  <si>
+    <t>7_09Oct23</t>
+  </si>
+  <si>
+    <t>8_09Oct23</t>
+  </si>
+  <si>
+    <t>1_24Oct23</t>
+  </si>
+  <si>
+    <t>2_24Oct23</t>
+  </si>
+  <si>
+    <t>3_24Oct23</t>
+  </si>
+  <si>
+    <t>4_24Oct23</t>
+  </si>
+  <si>
+    <t>5_24Oct23</t>
+  </si>
+  <si>
+    <t>6_24Oct23</t>
+  </si>
+  <si>
+    <t>7_24Oct23</t>
+  </si>
+  <si>
+    <t>8_24Oct23</t>
+  </si>
+  <si>
+    <t>1_06Nov23</t>
+  </si>
+  <si>
+    <t>2_06Nov23</t>
+  </si>
+  <si>
+    <t>3_06Nov23</t>
+  </si>
+  <si>
+    <t>4_06Nov23</t>
+  </si>
+  <si>
+    <t>5_06Nov23</t>
+  </si>
+  <si>
+    <t>6_06Nov23</t>
+  </si>
+  <si>
+    <t>7_06Nov23</t>
+  </si>
+  <si>
+    <t>8_06Nov23</t>
+  </si>
+  <si>
+    <t>1_17Nov23</t>
+  </si>
+  <si>
+    <t>2_17Nov23</t>
+  </si>
+  <si>
+    <t>3_17Nov23</t>
+  </si>
+  <si>
+    <t>4_17Nov23</t>
+  </si>
+  <si>
+    <t>5_17Nov23</t>
+  </si>
+  <si>
+    <t>6_17Nov23</t>
+  </si>
+  <si>
+    <t>7_17Nov23</t>
+  </si>
+  <si>
+    <t>8_17Nov23</t>
+  </si>
+  <si>
+    <t>5_04Dec23</t>
+  </si>
+  <si>
+    <t>6_04Dec23</t>
+  </si>
+  <si>
+    <t>7_04Dec23</t>
+  </si>
+  <si>
+    <t>8_04Dec23</t>
+  </si>
+  <si>
+    <t>1_04Dec23</t>
+  </si>
+  <si>
+    <t>2_04Dec23</t>
+  </si>
+  <si>
+    <t>3_04Dec23</t>
+  </si>
+  <si>
+    <t>4_04Dec23</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2159,7 @@
   <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2179,13 +2179,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>405</v>
+        <v>269</v>
       </c>
       <c r="E1" t="s">
-        <v>406</v>
+        <v>270</v>
       </c>
       <c r="F1" t="s">
-        <v>407</v>
+        <v>271</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -2194,27 +2194,27 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>415</v>
+        <v>279</v>
       </c>
       <c r="J1" t="s">
-        <v>408</v>
+        <v>272</v>
       </c>
       <c r="K1" t="s">
-        <v>409</v>
+        <v>273</v>
       </c>
       <c r="L1" t="s">
-        <v>410</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2243,13 +2243,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <f>D2+1</f>
@@ -2280,13 +2280,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D67" si="0">D3+1</f>
@@ -2317,13 +2317,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -2354,13 +2354,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>288</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -2391,13 +2391,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>290</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -2465,13 +2465,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -2502,13 +2502,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -2576,13 +2576,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>294</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -2650,13 +2650,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>296</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>402</v>
+        <v>266</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -2687,13 +2687,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>297</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -2724,13 +2724,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>298</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -2761,13 +2761,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>299</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>300</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -2835,13 +2835,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>301</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -2872,13 +2872,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>302</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -2909,13 +2909,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>304</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -2983,13 +2983,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>305</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -3020,13 +3020,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>306</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -3057,13 +3057,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>307</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -3094,13 +3094,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>308</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -3131,13 +3131,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>309</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -3168,13 +3168,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>310</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
@@ -3205,13 +3205,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>311</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -3242,13 +3242,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>312</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -3279,13 +3279,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>313</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
@@ -3316,10 +3316,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>413</v>
+        <v>277</v>
       </c>
       <c r="B32" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
@@ -3341,10 +3341,10 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="B33" t="s">
-        <v>412</v>
+        <v>276</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
@@ -3366,13 +3366,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>314</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
@@ -3403,13 +3403,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>315</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
@@ -3440,13 +3440,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
@@ -3514,13 +3514,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>318</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
@@ -3551,13 +3551,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
@@ -3588,13 +3588,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>320</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
@@ -3625,13 +3625,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>321</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
@@ -3662,13 +3662,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>118</v>
+        <v>322</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
@@ -3699,13 +3699,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>323</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
@@ -3736,13 +3736,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>324</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
@@ -3773,13 +3773,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>325</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
@@ -3810,13 +3810,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>326</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -3847,13 +3847,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>327</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
@@ -3884,13 +3884,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>328</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
@@ -3921,13 +3921,13 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>329</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
@@ -3958,13 +3958,13 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>330</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
@@ -3995,13 +3995,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>331</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
@@ -4032,13 +4032,13 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>332</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
@@ -4069,13 +4069,13 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
@@ -4106,13 +4106,13 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>334</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
@@ -4143,13 +4143,13 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>335</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
@@ -4180,13 +4180,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>336</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
@@ -4217,13 +4217,13 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>337</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
@@ -4254,13 +4254,13 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>338</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
@@ -4291,13 +4291,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>339</v>
       </c>
       <c r="B59" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
@@ -4328,13 +4328,13 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s">
-        <v>173</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>174</v>
+        <v>117</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
@@ -4365,13 +4365,13 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>341</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="D61">
         <f t="shared" si="0"/>
@@ -4402,13 +4402,13 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>342</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>121</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
@@ -4439,13 +4439,13 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>181</v>
+        <v>343</v>
       </c>
       <c r="B63" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
@@ -4476,13 +4476,13 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>184</v>
+        <v>344</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="C64" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
@@ -4513,13 +4513,13 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>187</v>
+        <v>345</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
@@ -4550,13 +4550,13 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>346</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
@@ -4587,13 +4587,13 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>347</v>
       </c>
       <c r="B67" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="D67">
         <f t="shared" si="0"/>
@@ -4624,13 +4624,13 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>133</v>
       </c>
       <c r="D68">
         <f t="shared" ref="D68:D131" si="2">D67+1</f>
@@ -4661,13 +4661,13 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>349</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="D69">
         <f t="shared" si="2"/>
@@ -4698,13 +4698,13 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>350</v>
       </c>
       <c r="B70" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>137</v>
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
@@ -4735,13 +4735,13 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>205</v>
+        <v>351</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="D71">
         <f t="shared" si="2"/>
@@ -4772,10 +4772,10 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>413</v>
+        <v>277</v>
       </c>
       <c r="B72" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
       <c r="D72">
         <f t="shared" si="2"/>
@@ -4797,10 +4797,10 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="B73" t="s">
-        <v>412</v>
+        <v>276</v>
       </c>
       <c r="D73">
         <f t="shared" si="2"/>
@@ -4822,13 +4822,13 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>208</v>
+        <v>352</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="C74" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="D74">
         <f t="shared" si="2"/>
@@ -4859,13 +4859,13 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>353</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
       <c r="C75" t="s">
-        <v>213</v>
+        <v>143</v>
       </c>
       <c r="D75">
         <f t="shared" si="2"/>
@@ -4896,13 +4896,13 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>214</v>
+        <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="C76" t="s">
-        <v>216</v>
+        <v>145</v>
       </c>
       <c r="D76">
         <f t="shared" si="2"/>
@@ -4933,13 +4933,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>217</v>
+        <v>355</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="C77" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="D77">
         <f t="shared" si="2"/>
@@ -4970,13 +4970,13 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>220</v>
+        <v>356</v>
       </c>
       <c r="B78" t="s">
-        <v>221</v>
+        <v>148</v>
       </c>
       <c r="C78" t="s">
-        <v>222</v>
+        <v>149</v>
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
@@ -5007,13 +5007,13 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>223</v>
+        <v>357</v>
       </c>
       <c r="B79" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
@@ -5044,13 +5044,13 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>226</v>
+        <v>358</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>152</v>
       </c>
       <c r="C80" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="D80">
         <f t="shared" si="2"/>
@@ -5081,13 +5081,13 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>229</v>
+        <v>359</v>
       </c>
       <c r="B81" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="D81">
         <f t="shared" si="2"/>
@@ -5118,13 +5118,13 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>232</v>
+        <v>360</v>
       </c>
       <c r="B82" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
       <c r="C82" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
@@ -5155,13 +5155,13 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>235</v>
+        <v>361</v>
       </c>
       <c r="B83" t="s">
-        <v>236</v>
+        <v>158</v>
       </c>
       <c r="C83" t="s">
-        <v>237</v>
+        <v>159</v>
       </c>
       <c r="D83">
         <f t="shared" si="2"/>
@@ -5192,13 +5192,13 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>362</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>160</v>
       </c>
       <c r="C84" t="s">
-        <v>240</v>
+        <v>161</v>
       </c>
       <c r="D84">
         <f t="shared" si="2"/>
@@ -5229,13 +5229,13 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>241</v>
+        <v>363</v>
       </c>
       <c r="B85" t="s">
-        <v>242</v>
+        <v>162</v>
       </c>
       <c r="C85" t="s">
-        <v>243</v>
+        <v>163</v>
       </c>
       <c r="D85">
         <f t="shared" si="2"/>
@@ -5266,13 +5266,13 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>164</v>
       </c>
       <c r="C86" t="s">
-        <v>246</v>
+        <v>165</v>
       </c>
       <c r="D86">
         <f t="shared" si="2"/>
@@ -5303,13 +5303,13 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>247</v>
+        <v>365</v>
       </c>
       <c r="B87" t="s">
-        <v>248</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>249</v>
+        <v>167</v>
       </c>
       <c r="D87">
         <f t="shared" si="2"/>
@@ -5340,13 +5340,13 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>366</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>168</v>
       </c>
       <c r="C88" t="s">
-        <v>252</v>
+        <v>169</v>
       </c>
       <c r="D88">
         <f t="shared" si="2"/>
@@ -5377,13 +5377,13 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>253</v>
+        <v>367</v>
       </c>
       <c r="B89" t="s">
-        <v>254</v>
+        <v>170</v>
       </c>
       <c r="C89" t="s">
-        <v>255</v>
+        <v>171</v>
       </c>
       <c r="D89">
         <f t="shared" si="2"/>
@@ -5414,13 +5414,13 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>256</v>
+        <v>368</v>
       </c>
       <c r="B90" t="s">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="C90" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
       <c r="D90">
         <f t="shared" si="2"/>
@@ -5451,13 +5451,13 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>259</v>
+        <v>369</v>
       </c>
       <c r="B91" t="s">
-        <v>260</v>
+        <v>174</v>
       </c>
       <c r="C91" t="s">
-        <v>261</v>
+        <v>175</v>
       </c>
       <c r="D91">
         <f t="shared" si="2"/>
@@ -5488,13 +5488,13 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B92" t="s">
-        <v>263</v>
+        <v>176</v>
       </c>
       <c r="C92" t="s">
-        <v>264</v>
+        <v>177</v>
       </c>
       <c r="D92">
         <f t="shared" si="2"/>
@@ -5525,13 +5525,13 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>265</v>
+        <v>371</v>
       </c>
       <c r="B93" t="s">
-        <v>266</v>
+        <v>178</v>
       </c>
       <c r="C93" t="s">
-        <v>267</v>
+        <v>179</v>
       </c>
       <c r="D93">
         <f t="shared" si="2"/>
@@ -5562,13 +5562,13 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>268</v>
+        <v>372</v>
       </c>
       <c r="B94" t="s">
-        <v>269</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s">
-        <v>270</v>
+        <v>181</v>
       </c>
       <c r="D94">
         <f t="shared" si="2"/>
@@ -5599,13 +5599,13 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>271</v>
+        <v>373</v>
       </c>
       <c r="B95" t="s">
-        <v>272</v>
+        <v>182</v>
       </c>
       <c r="C95" t="s">
-        <v>273</v>
+        <v>183</v>
       </c>
       <c r="D95">
         <f t="shared" si="2"/>
@@ -5636,13 +5636,13 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>274</v>
+        <v>374</v>
       </c>
       <c r="B96" t="s">
-        <v>275</v>
+        <v>184</v>
       </c>
       <c r="C96" t="s">
-        <v>276</v>
+        <v>185</v>
       </c>
       <c r="D96">
         <f t="shared" si="2"/>
@@ -5673,13 +5673,13 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>375</v>
       </c>
       <c r="B97" t="s">
-        <v>278</v>
+        <v>186</v>
       </c>
       <c r="C97" t="s">
-        <v>279</v>
+        <v>187</v>
       </c>
       <c r="D97">
         <f t="shared" si="2"/>
@@ -5710,10 +5710,10 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>413</v>
+        <v>277</v>
       </c>
       <c r="B98" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
       <c r="D98">
         <f t="shared" si="2"/>
@@ -5735,10 +5735,10 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="B99" t="s">
-        <v>412</v>
+        <v>276</v>
       </c>
       <c r="D99">
         <f t="shared" si="2"/>
@@ -5760,13 +5760,13 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>280</v>
+        <v>377</v>
       </c>
       <c r="B100" t="s">
-        <v>281</v>
+        <v>188</v>
       </c>
       <c r="C100" t="s">
-        <v>282</v>
+        <v>189</v>
       </c>
       <c r="D100">
         <f t="shared" si="2"/>
@@ -5797,13 +5797,13 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>283</v>
+        <v>376</v>
       </c>
       <c r="B101" t="s">
-        <v>284</v>
+        <v>190</v>
       </c>
       <c r="C101" t="s">
-        <v>285</v>
+        <v>191</v>
       </c>
       <c r="D101">
         <f t="shared" si="2"/>
@@ -5834,13 +5834,13 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>286</v>
+        <v>378</v>
       </c>
       <c r="B102" t="s">
-        <v>287</v>
+        <v>192</v>
       </c>
       <c r="C102" t="s">
-        <v>288</v>
+        <v>193</v>
       </c>
       <c r="D102">
         <f t="shared" si="2"/>
@@ -5871,13 +5871,13 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>289</v>
+        <v>379</v>
       </c>
       <c r="B103" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="C103" t="s">
-        <v>291</v>
+        <v>195</v>
       </c>
       <c r="D103">
         <f t="shared" si="2"/>
@@ -5908,13 +5908,13 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>292</v>
+        <v>380</v>
       </c>
       <c r="B104" t="s">
-        <v>293</v>
+        <v>196</v>
       </c>
       <c r="C104" t="s">
-        <v>294</v>
+        <v>197</v>
       </c>
       <c r="D104">
         <f t="shared" si="2"/>
@@ -5945,13 +5945,13 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>295</v>
+        <v>381</v>
       </c>
       <c r="B105" t="s">
-        <v>296</v>
+        <v>198</v>
       </c>
       <c r="C105" t="s">
-        <v>297</v>
+        <v>199</v>
       </c>
       <c r="D105">
         <f t="shared" si="2"/>
@@ -5982,13 +5982,13 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>298</v>
+        <v>382</v>
       </c>
       <c r="B106" t="s">
-        <v>299</v>
+        <v>200</v>
       </c>
       <c r="C106" t="s">
-        <v>300</v>
+        <v>201</v>
       </c>
       <c r="D106">
         <f t="shared" si="2"/>
@@ -6019,13 +6019,13 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>301</v>
+        <v>383</v>
       </c>
       <c r="B107" t="s">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="C107" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="D107">
         <f t="shared" si="2"/>
@@ -6056,13 +6056,13 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>384</v>
       </c>
       <c r="B108" t="s">
-        <v>305</v>
+        <v>204</v>
       </c>
       <c r="C108" t="s">
-        <v>306</v>
+        <v>205</v>
       </c>
       <c r="D108">
         <f t="shared" si="2"/>
@@ -6093,13 +6093,13 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>307</v>
+        <v>385</v>
       </c>
       <c r="B109" t="s">
-        <v>308</v>
+        <v>206</v>
       </c>
       <c r="C109" t="s">
-        <v>309</v>
+        <v>207</v>
       </c>
       <c r="D109">
         <f t="shared" si="2"/>
@@ -6130,13 +6130,13 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>310</v>
+        <v>386</v>
       </c>
       <c r="B110" t="s">
-        <v>311</v>
+        <v>208</v>
       </c>
       <c r="C110" t="s">
-        <v>312</v>
+        <v>209</v>
       </c>
       <c r="D110">
         <f t="shared" si="2"/>
@@ -6167,13 +6167,13 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>313</v>
+        <v>387</v>
       </c>
       <c r="B111" t="s">
-        <v>314</v>
+        <v>210</v>
       </c>
       <c r="C111" t="s">
-        <v>315</v>
+        <v>211</v>
       </c>
       <c r="D111">
         <f t="shared" si="2"/>
@@ -6204,13 +6204,13 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>316</v>
+        <v>388</v>
       </c>
       <c r="B112" t="s">
-        <v>317</v>
+        <v>212</v>
       </c>
       <c r="C112" t="s">
-        <v>318</v>
+        <v>213</v>
       </c>
       <c r="D112">
         <f t="shared" si="2"/>
@@ -6241,13 +6241,13 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>319</v>
+        <v>389</v>
       </c>
       <c r="B113" t="s">
-        <v>320</v>
+        <v>214</v>
       </c>
       <c r="C113" t="s">
-        <v>321</v>
+        <v>215</v>
       </c>
       <c r="D113">
         <f t="shared" si="2"/>
@@ -6278,13 +6278,13 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>322</v>
+        <v>390</v>
       </c>
       <c r="B114" t="s">
-        <v>323</v>
+        <v>216</v>
       </c>
       <c r="C114" t="s">
-        <v>324</v>
+        <v>217</v>
       </c>
       <c r="D114">
         <f t="shared" si="2"/>
@@ -6315,13 +6315,13 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>325</v>
+        <v>391</v>
       </c>
       <c r="B115" t="s">
-        <v>326</v>
+        <v>218</v>
       </c>
       <c r="C115" t="s">
-        <v>327</v>
+        <v>219</v>
       </c>
       <c r="D115">
         <f t="shared" si="2"/>
@@ -6352,13 +6352,13 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>328</v>
+        <v>392</v>
       </c>
       <c r="B116" t="s">
-        <v>329</v>
+        <v>220</v>
       </c>
       <c r="C116" t="s">
-        <v>330</v>
+        <v>221</v>
       </c>
       <c r="D116">
         <f t="shared" si="2"/>
@@ -6389,13 +6389,13 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>393</v>
       </c>
       <c r="B117" t="s">
-        <v>332</v>
+        <v>222</v>
       </c>
       <c r="C117" t="s">
-        <v>333</v>
+        <v>223</v>
       </c>
       <c r="D117">
         <f t="shared" si="2"/>
@@ -6426,13 +6426,13 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>334</v>
+        <v>394</v>
       </c>
       <c r="B118" t="s">
-        <v>335</v>
+        <v>224</v>
       </c>
       <c r="C118" t="s">
-        <v>336</v>
+        <v>225</v>
       </c>
       <c r="D118">
         <f t="shared" si="2"/>
@@ -6463,13 +6463,13 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>337</v>
+        <v>395</v>
       </c>
       <c r="B119" t="s">
-        <v>338</v>
+        <v>226</v>
       </c>
       <c r="C119" t="s">
-        <v>339</v>
+        <v>227</v>
       </c>
       <c r="D119">
         <f t="shared" si="2"/>
@@ -6500,13 +6500,13 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="B120" t="s">
-        <v>341</v>
+        <v>228</v>
       </c>
       <c r="C120" t="s">
-        <v>342</v>
+        <v>229</v>
       </c>
       <c r="D120">
         <f t="shared" si="2"/>
@@ -6537,13 +6537,13 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="B121" t="s">
-        <v>344</v>
+        <v>230</v>
       </c>
       <c r="C121" t="s">
-        <v>345</v>
+        <v>231</v>
       </c>
       <c r="D121">
         <f t="shared" si="2"/>
@@ -6574,13 +6574,13 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="B122" t="s">
-        <v>344</v>
+        <v>230</v>
       </c>
       <c r="C122" t="s">
-        <v>345</v>
+        <v>231</v>
       </c>
       <c r="D122">
         <f t="shared" si="2"/>
@@ -6611,13 +6611,13 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>346</v>
+        <v>398</v>
       </c>
       <c r="B123" t="s">
-        <v>347</v>
+        <v>232</v>
       </c>
       <c r="C123" t="s">
-        <v>348</v>
+        <v>233</v>
       </c>
       <c r="D123">
         <f t="shared" si="2"/>
@@ -6648,13 +6648,13 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>349</v>
+        <v>399</v>
       </c>
       <c r="B124" t="s">
-        <v>350</v>
+        <v>234</v>
       </c>
       <c r="C124" t="s">
-        <v>403</v>
+        <v>267</v>
       </c>
       <c r="D124">
         <f t="shared" si="2"/>
@@ -6685,13 +6685,13 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>351</v>
+        <v>400</v>
       </c>
       <c r="B125" t="s">
-        <v>352</v>
+        <v>235</v>
       </c>
       <c r="C125" t="s">
-        <v>353</v>
+        <v>236</v>
       </c>
       <c r="D125">
         <f t="shared" si="2"/>
@@ -6722,13 +6722,13 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>354</v>
+        <v>401</v>
       </c>
       <c r="B126" t="s">
-        <v>355</v>
+        <v>237</v>
       </c>
       <c r="C126" t="s">
-        <v>356</v>
+        <v>238</v>
       </c>
       <c r="D126">
         <f t="shared" si="2"/>
@@ -6759,13 +6759,13 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>357</v>
+        <v>402</v>
       </c>
       <c r="B127" t="s">
-        <v>358</v>
+        <v>239</v>
       </c>
       <c r="C127" t="s">
-        <v>359</v>
+        <v>240</v>
       </c>
       <c r="D127">
         <f t="shared" si="2"/>
@@ -6796,13 +6796,13 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="B128" t="s">
-        <v>361</v>
+        <v>241</v>
       </c>
       <c r="C128" t="s">
-        <v>362</v>
+        <v>242</v>
       </c>
       <c r="D128">
         <f t="shared" si="2"/>
@@ -6833,13 +6833,13 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>363</v>
+        <v>404</v>
       </c>
       <c r="B129" t="s">
-        <v>364</v>
+        <v>243</v>
       </c>
       <c r="C129" t="s">
-        <v>365</v>
+        <v>244</v>
       </c>
       <c r="D129">
         <f t="shared" si="2"/>
@@ -6870,13 +6870,13 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="B130" t="s">
-        <v>367</v>
+        <v>245</v>
       </c>
       <c r="C130" t="s">
-        <v>368</v>
+        <v>246</v>
       </c>
       <c r="D130">
         <f t="shared" si="2"/>
@@ -6907,13 +6907,13 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="B131" t="s">
-        <v>367</v>
+        <v>245</v>
       </c>
       <c r="C131" t="s">
-        <v>368</v>
+        <v>246</v>
       </c>
       <c r="D131">
         <f t="shared" si="2"/>
@@ -6944,13 +6944,13 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>369</v>
+        <v>406</v>
       </c>
       <c r="B132" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="C132" t="s">
-        <v>371</v>
+        <v>248</v>
       </c>
       <c r="D132">
         <f t="shared" ref="D132:D149" si="4">D131+1</f>
@@ -6981,13 +6981,13 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
       <c r="B133" t="s">
-        <v>373</v>
+        <v>249</v>
       </c>
       <c r="C133" t="s">
-        <v>404</v>
+        <v>268</v>
       </c>
       <c r="D133">
         <f t="shared" si="4"/>
@@ -7018,10 +7018,10 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>413</v>
+        <v>277</v>
       </c>
       <c r="B134" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
       <c r="D134">
         <f t="shared" si="4"/>
@@ -7043,10 +7043,10 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="B135" t="s">
-        <v>412</v>
+        <v>276</v>
       </c>
       <c r="D135">
         <f t="shared" si="4"/>
@@ -7068,13 +7068,13 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
       <c r="B136" t="s">
-        <v>375</v>
+        <v>250</v>
       </c>
       <c r="C136" t="s">
-        <v>376</v>
+        <v>251</v>
       </c>
       <c r="D136">
         <f t="shared" si="4"/>
@@ -7105,13 +7105,13 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c r="B137" t="s">
-        <v>378</v>
+        <v>252</v>
       </c>
       <c r="C137" t="s">
-        <v>379</v>
+        <v>253</v>
       </c>
       <c r="D137">
         <f t="shared" si="4"/>
@@ -7142,10 +7142,10 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>380</v>
+        <v>410</v>
       </c>
       <c r="B138" t="s">
-        <v>416</v>
+        <v>280</v>
       </c>
       <c r="D138">
         <f t="shared" si="4"/>
@@ -7173,10 +7173,10 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>381</v>
+        <v>411</v>
       </c>
       <c r="B139" t="s">
-        <v>417</v>
+        <v>281</v>
       </c>
       <c r="D139">
         <f t="shared" si="4"/>
@@ -7204,10 +7204,10 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>382</v>
+        <v>412</v>
       </c>
       <c r="B140" t="s">
-        <v>418</v>
+        <v>282</v>
       </c>
       <c r="D140">
         <f t="shared" si="4"/>
@@ -7235,13 +7235,13 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>383</v>
+        <v>413</v>
       </c>
       <c r="B141" t="s">
-        <v>384</v>
+        <v>254</v>
       </c>
       <c r="C141" t="s">
-        <v>385</v>
+        <v>255</v>
       </c>
       <c r="D141">
         <f t="shared" si="4"/>
@@ -7272,13 +7272,13 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>386</v>
+        <v>414</v>
       </c>
       <c r="B142" t="s">
-        <v>387</v>
+        <v>256</v>
       </c>
       <c r="C142" t="s">
-        <v>388</v>
+        <v>257</v>
       </c>
       <c r="D142">
         <f t="shared" si="4"/>
@@ -7309,13 +7309,13 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="B143" t="s">
-        <v>390</v>
+        <v>258</v>
       </c>
       <c r="C143" t="s">
-        <v>391</v>
+        <v>259</v>
       </c>
       <c r="D143">
         <f t="shared" si="4"/>
@@ -7346,10 +7346,10 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>392</v>
+        <v>416</v>
       </c>
       <c r="B144" t="s">
-        <v>419</v>
+        <v>283</v>
       </c>
       <c r="D144">
         <f t="shared" si="4"/>
@@ -7377,13 +7377,13 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="B145" t="s">
-        <v>394</v>
+        <v>260</v>
       </c>
       <c r="C145" t="s">
-        <v>395</v>
+        <v>261</v>
       </c>
       <c r="D145">
         <f t="shared" si="4"/>
@@ -7414,13 +7414,13 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="B146" t="s">
-        <v>397</v>
+        <v>262</v>
       </c>
       <c r="C146" t="s">
-        <v>398</v>
+        <v>263</v>
       </c>
       <c r="D146">
         <f t="shared" si="4"/>
@@ -7451,13 +7451,13 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="B147" t="s">
-        <v>400</v>
+        <v>264</v>
       </c>
       <c r="C147" t="s">
-        <v>401</v>
+        <v>265</v>
       </c>
       <c r="D147">
         <f t="shared" si="4"/>
@@ -7488,10 +7488,10 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>413</v>
+        <v>277</v>
       </c>
       <c r="B148" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
       <c r="D148">
         <f t="shared" si="4"/>
@@ -7513,10 +7513,10 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>414</v>
+        <v>278</v>
       </c>
       <c r="B149" t="s">
-        <v>412</v>
+        <v>276</v>
       </c>
       <c r="D149">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
noticed duplicates so had to change some things
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2023_AcidDigestion_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/2023_AcidDigestion_EDI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Metals/Digestions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD035BB5-47DF-034F-BEE3-441A3F430E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F25A225-F939-F742-886E-ABE0B7B5F137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15500" xr2:uid="{09F8E85E-FD52-2D49-8A5D-8718B1783EFE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="442" uniqueCount="420">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="436" uniqueCount="420">
   <si>
     <t>Sample</t>
   </si>
@@ -2156,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD420553-E4B0-0F4E-AA03-3DCACE68954F}">
-  <dimension ref="A1:L149"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6574,13 +6574,13 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B122" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C122" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D122">
         <f t="shared" si="2"/>
@@ -6591,10 +6591,10 @@
         <v>121</v>
       </c>
       <c r="G122">
-        <v>1.6E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H122">
-        <v>3.6999999999999998E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I122">
         <v>0.01</v>
@@ -6611,13 +6611,13 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B123" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C123" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="D123">
         <f t="shared" si="2"/>
@@ -6628,10 +6628,10 @@
         <v>122</v>
       </c>
       <c r="G123">
-        <v>2.5000000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="H123">
-        <v>2.5000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I123">
         <v>0.01</v>
@@ -6648,13 +6648,13 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B124" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C124" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
       <c r="D124">
         <f t="shared" si="2"/>
@@ -6665,10 +6665,10 @@
         <v>123</v>
       </c>
       <c r="G124">
-        <v>3.4000000000000002E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H124">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I124">
         <v>0.01</v>
@@ -6685,13 +6685,13 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B125" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C125" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D125">
         <f t="shared" si="2"/>
@@ -6702,10 +6702,10 @@
         <v>124</v>
       </c>
       <c r="G125">
-        <v>1.9E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H125">
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I125">
         <v>0.01</v>
@@ -6722,13 +6722,13 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B126" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C126" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D126">
         <f t="shared" si="2"/>
@@ -6739,10 +6739,10 @@
         <v>125</v>
       </c>
       <c r="G126">
+        <v>0.01</v>
+      </c>
+      <c r="H126">
         <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H126">
-        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I126">
         <v>0.01</v>
@@ -6759,13 +6759,13 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B127" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C127" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D127">
         <f t="shared" si="2"/>
@@ -6776,10 +6776,10 @@
         <v>126</v>
       </c>
       <c r="G127">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H127">
-        <v>8.0000000000000002E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I127">
         <v>0.01</v>
@@ -6796,13 +6796,13 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C128" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D128">
         <f t="shared" si="2"/>
@@ -6813,10 +6813,10 @@
         <v>127</v>
       </c>
       <c r="G128">
-        <v>8.9999999999999993E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H128">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I128">
         <v>0.01</v>
@@ -6828,18 +6828,18 @@
         <v>0.01</v>
       </c>
       <c r="L128">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B129" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C129" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D129">
         <f t="shared" si="2"/>
@@ -6850,10 +6850,10 @@
         <v>128</v>
       </c>
       <c r="G129">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H129">
         <v>1.2E-2</v>
-      </c>
-      <c r="H129">
-        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I129">
         <v>0.01</v>
@@ -6870,13 +6870,13 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B130" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C130" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D130">
         <f t="shared" si="2"/>
@@ -6887,10 +6887,10 @@
         <v>129</v>
       </c>
       <c r="G130">
-        <v>1.0999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H130">
-        <v>1.2E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="I130">
         <v>0.01</v>
@@ -6907,13 +6907,13 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B131" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C131" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="D131">
         <f t="shared" si="2"/>
@@ -6924,10 +6924,10 @@
         <v>130</v>
       </c>
       <c r="G131">
-        <v>1.0999999999999999E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H131">
-        <v>2.4E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I131">
         <v>0.01</v>
@@ -6944,28 +6944,19 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>406</v>
+        <v>277</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
-      </c>
-      <c r="C132" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="D132">
-        <f t="shared" ref="D132:D149" si="4">D131+1</f>
+        <f t="shared" ref="D132:D147" si="4">D131+1</f>
         <v>131</v>
       </c>
       <c r="F132">
-        <f t="shared" ref="F132:F149" si="5">F131+1</f>
+        <f t="shared" ref="F132:F147" si="5">F131+1</f>
         <v>131</v>
       </c>
-      <c r="G132">
-        <v>2.7E-2</v>
-      </c>
-      <c r="H132">
-        <v>2.7E-2</v>
-      </c>
       <c r="I132">
         <v>0.01</v>
       </c>
@@ -6974,20 +6965,14 @@
       </c>
       <c r="K132">
         <v>0.01</v>
-      </c>
-      <c r="L132">
-        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>407</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>249</v>
-      </c>
-      <c r="C133" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D133">
         <f t="shared" si="4"/>
@@ -6997,12 +6982,6 @@
         <f t="shared" si="5"/>
         <v>132</v>
       </c>
-      <c r="G133">
-        <v>2.4E-2</v>
-      </c>
-      <c r="H133">
-        <v>8.0000000000000002E-3</v>
-      </c>
       <c r="I133">
         <v>0.01</v>
       </c>
@@ -7011,17 +6990,17 @@
       </c>
       <c r="K133">
         <v>0.01</v>
-      </c>
-      <c r="L133">
-        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>277</v>
+        <v>408</v>
       </c>
       <c r="B134" t="s">
-        <v>275</v>
+        <v>250</v>
+      </c>
+      <c r="C134" t="s">
+        <v>251</v>
       </c>
       <c r="D134">
         <f t="shared" si="4"/>
@@ -7031,6 +7010,12 @@
         <f t="shared" si="5"/>
         <v>133</v>
       </c>
+      <c r="G134">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H134">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="I134">
         <v>0.01</v>
       </c>
@@ -7039,14 +7024,20 @@
       </c>
       <c r="K134">
         <v>0.01</v>
+      </c>
+      <c r="L134">
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>278</v>
+        <v>409</v>
       </c>
       <c r="B135" t="s">
-        <v>276</v>
+        <v>252</v>
+      </c>
+      <c r="C135" t="s">
+        <v>253</v>
       </c>
       <c r="D135">
         <f t="shared" si="4"/>
@@ -7056,6 +7047,12 @@
         <f t="shared" si="5"/>
         <v>134</v>
       </c>
+      <c r="G135">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H135">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="I135">
         <v>0.01</v>
       </c>
@@ -7064,17 +7061,17 @@
       </c>
       <c r="K135">
         <v>0.01</v>
+      </c>
+      <c r="L135">
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B136" t="s">
-        <v>250</v>
-      </c>
-      <c r="C136" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="D136">
         <f t="shared" si="4"/>
@@ -7085,9 +7082,6 @@
         <v>135</v>
       </c>
       <c r="G136">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H136">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="I136">
@@ -7105,13 +7099,10 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
-      </c>
-      <c r="C137" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="D137">
         <f t="shared" si="4"/>
@@ -7122,10 +7113,7 @@
         <v>136</v>
       </c>
       <c r="G137">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H137">
-        <v>4.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I137">
         <v>0.01</v>
@@ -7142,10 +7130,10 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B138" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D138">
         <f t="shared" si="4"/>
@@ -7156,7 +7144,7 @@
         <v>137</v>
       </c>
       <c r="G138">
-        <v>6.0000000000000001E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I138">
         <v>0.01</v>
@@ -7168,15 +7156,18 @@
         <v>0.01</v>
       </c>
       <c r="L138">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B139" t="s">
-        <v>281</v>
+        <v>254</v>
+      </c>
+      <c r="C139" t="s">
+        <v>255</v>
       </c>
       <c r="D139">
         <f t="shared" si="4"/>
@@ -7187,7 +7178,10 @@
         <v>138</v>
       </c>
       <c r="G139">
-        <v>6.0000000000000001E-3</v>
+        <v>1.2E-2</v>
+      </c>
+      <c r="H139">
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I139">
         <v>0.01</v>
@@ -7199,15 +7193,18 @@
         <v>0.01</v>
       </c>
       <c r="L139">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B140" t="s">
-        <v>282</v>
+        <v>256</v>
+      </c>
+      <c r="C140" t="s">
+        <v>257</v>
       </c>
       <c r="D140">
         <f t="shared" si="4"/>
@@ -7218,7 +7215,10 @@
         <v>139</v>
       </c>
       <c r="G140">
-        <v>1.0999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H140">
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I140">
         <v>0.01</v>
@@ -7235,13 +7235,13 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B141" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C141" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D141">
         <f t="shared" si="4"/>
@@ -7252,10 +7252,10 @@
         <v>140</v>
       </c>
       <c r="G141">
-        <v>1.2E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H141">
-        <v>1.2999999999999999E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I141">
         <v>0.01</v>
@@ -7272,13 +7272,10 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B142" t="s">
-        <v>256</v>
-      </c>
-      <c r="C142" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="D142">
         <f t="shared" si="4"/>
@@ -7289,10 +7286,7 @@
         <v>141</v>
       </c>
       <c r="G142">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="H142">
-        <v>1.2999999999999999E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I142">
         <v>0.01</v>
@@ -7309,13 +7303,13 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B143" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C143" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D143">
         <f t="shared" si="4"/>
@@ -7326,10 +7320,10 @@
         <v>142</v>
       </c>
       <c r="G143">
-        <v>0.01</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H143">
-        <v>1.0999999999999999E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I143">
         <v>0.01</v>
@@ -7346,10 +7340,13 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B144" t="s">
-        <v>283</v>
+        <v>262</v>
+      </c>
+      <c r="C144" t="s">
+        <v>263</v>
       </c>
       <c r="D144">
         <f t="shared" si="4"/>
@@ -7360,7 +7357,10 @@
         <v>143</v>
       </c>
       <c r="G144">
-        <v>2.5999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H144">
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="I144">
         <v>0.01</v>
@@ -7377,13 +7377,13 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B145" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C145" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D145">
         <f t="shared" si="4"/>
@@ -7394,10 +7394,10 @@
         <v>144</v>
       </c>
       <c r="G145">
-        <v>2.8000000000000001E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="H145">
-        <v>2.5999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="I145">
         <v>0.01</v>
@@ -7414,13 +7414,10 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>418</v>
+        <v>277</v>
       </c>
       <c r="B146" t="s">
-        <v>262</v>
-      </c>
-      <c r="C146" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="D146">
         <f t="shared" si="4"/>
@@ -7430,12 +7427,6 @@
         <f t="shared" si="5"/>
         <v>145</v>
       </c>
-      <c r="G146">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="H146">
-        <v>3.3000000000000002E-2</v>
-      </c>
       <c r="I146">
         <v>0.01</v>
       </c>
@@ -7444,20 +7435,14 @@
       </c>
       <c r="K146">
         <v>0.01</v>
-      </c>
-      <c r="L146">
-        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>419</v>
+        <v>278</v>
       </c>
       <c r="B147" t="s">
-        <v>264</v>
-      </c>
-      <c r="C147" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="D147">
         <f t="shared" si="4"/>
@@ -7467,12 +7452,6 @@
         <f t="shared" si="5"/>
         <v>146</v>
       </c>
-      <c r="G147">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="H147">
-        <v>3.3000000000000002E-2</v>
-      </c>
       <c r="I147">
         <v>0.01</v>
       </c>
@@ -7480,59 +7459,6 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="K147">
-        <v>0.01</v>
-      </c>
-      <c r="L147">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>277</v>
-      </c>
-      <c r="B148" t="s">
-        <v>275</v>
-      </c>
-      <c r="D148">
-        <f t="shared" si="4"/>
-        <v>147</v>
-      </c>
-      <c r="F148">
-        <f t="shared" si="5"/>
-        <v>147</v>
-      </c>
-      <c r="I148">
-        <v>0.01</v>
-      </c>
-      <c r="J148">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="K148">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>278</v>
-      </c>
-      <c r="B149" t="s">
-        <v>276</v>
-      </c>
-      <c r="D149">
-        <f t="shared" si="4"/>
-        <v>148</v>
-      </c>
-      <c r="F149">
-        <f t="shared" si="5"/>
-        <v>148</v>
-      </c>
-      <c r="I149">
-        <v>0.01</v>
-      </c>
-      <c r="J149">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="K149">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>